<commit_message>
files added by kavin
</commit_message>
<xml_diff>
--- a/cypress/fixtures/orange_excel.xlsx
+++ b/cypress/fixtures/orange_excel.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18600" windowHeight="6950"/>
+    <workbookView windowWidth="18600" windowHeight="6500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="Details" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <r>
       <rPr>
@@ -113,6 +114,54 @@
       </rPr>
       <t>Invalid credentials</t>
     </r>
+  </si>
+  <si>
+    <t>fullname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>comName</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>empCount</t>
+  </si>
+  <si>
+    <t>jobTitle</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>Demouser</t>
+  </si>
+  <si>
+    <t>demotest@gmail.com</t>
+  </si>
+  <si>
+    <t>demo</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Demo Test</t>
+  </si>
+  <si>
+    <t>Thank you.</t>
   </si>
 </sst>
 </file>
@@ -125,13 +174,18 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="Consolas"/>
+      <charset val="0"/>
     </font>
     <font>
       <b/>
@@ -606,64 +660,64 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -672,10 +726,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -684,10 +738,10 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -696,10 +750,10 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -708,10 +762,10 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -720,10 +774,10 @@
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -732,15 +786,24 @@
     <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1286,7 +1349,7 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1297,47 +1360,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="20.7272727272727" customWidth="1"/>
+    <col min="4" max="4" width="12.7272727272727"/>
+    <col min="6" max="6" width="12.3636363636364" customWidth="1"/>
+    <col min="7" max="7" width="11.4545454545455" customWidth="1"/>
+    <col min="8" max="8" width="10.8181818181818" customWidth="1"/>
+    <col min="9" max="9" width="13.9090909090909" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" ht="40.5" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2">
+        <v>6385667530</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45611</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>